<commit_message>
Added ability to have libraries internal to the program
</commit_message>
<xml_diff>
--- a/reportFile.xlsx
+++ b/reportFile.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Report Creation Date:</t>
   </si>
   <si>
-    <t>03/17/2016 22:57</t>
+    <t>03/25/2016 13:57</t>
   </si>
   <si>
     <t>Load Shed Controller Report</t>
@@ -39,6 +39,63 @@
   </si>
   <si>
     <t>Time Stamp</t>
+  </si>
+  <si>
+    <t>Ricky Martinez</t>
+  </si>
+  <si>
+    <t>Power Off</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:53:42</t>
+  </si>
+  <si>
+    <t>Power On</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:53:49</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:53:55</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:53:59</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:54:04</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:54:07</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:55:45</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:55:57</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:33</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:36</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:38</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:40</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:43</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:45</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:47</t>
+  </si>
+  <si>
+    <t>03/25/2016  13:56:49</t>
   </si>
 </sst>
 </file>
@@ -46,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="16">
+  <fonts count="80">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -114,6 +171,262 @@
       <name val="Calibri"/>
       <sz val="11.0"/>
       <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -175,7 +488,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
@@ -206,6 +519,199 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -241,7 +747,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" t="n" s="10">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -289,6 +795,255 @@
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="19"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="B11" s="21"/>
+      <c r="C11" t="s" s="23">
+        <v>10</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="28">
+        <v>9</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" t="s" s="29">
+        <v>12</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" t="s" s="30">
+        <v>13</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="31"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="34">
+        <v>9</v>
+      </c>
+      <c r="B13" s="33"/>
+      <c r="C13" t="s" s="35">
+        <v>10</v>
+      </c>
+      <c r="D13" s="33"/>
+      <c r="E13" t="s" s="36">
+        <v>14</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="37"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="40">
+        <v>9</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" t="s" s="41">
+        <v>12</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" t="s" s="42">
+        <v>15</v>
+      </c>
+      <c r="F14" s="39"/>
+      <c r="G14" s="43"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="46">
+        <v>9</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" t="s" s="47">
+        <v>10</v>
+      </c>
+      <c r="D15" s="45"/>
+      <c r="E15" t="s" s="48">
+        <v>16</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="G15" s="49"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="52">
+        <v>9</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" t="s" s="53">
+        <v>12</v>
+      </c>
+      <c r="D16" s="51"/>
+      <c r="E16" t="s" s="54">
+        <v>17</v>
+      </c>
+      <c r="F16" s="51"/>
+      <c r="G16" s="55"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s" s="58">
+        <v>9</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" t="s" s="59">
+        <v>10</v>
+      </c>
+      <c r="D17" s="57"/>
+      <c r="E17" t="s" s="60">
+        <v>18</v>
+      </c>
+      <c r="F17" s="57"/>
+      <c r="G17" s="61"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="64">
+        <v>9</v>
+      </c>
+      <c r="B18" s="63"/>
+      <c r="C18" t="s" s="65">
+        <v>12</v>
+      </c>
+      <c r="D18" s="63"/>
+      <c r="E18" t="s" s="66">
+        <v>19</v>
+      </c>
+      <c r="F18" s="63"/>
+      <c r="G18" s="67"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="70">
+        <v>9</v>
+      </c>
+      <c r="B19" s="69"/>
+      <c r="C19" t="s" s="71">
+        <v>10</v>
+      </c>
+      <c r="D19" s="69"/>
+      <c r="E19" t="s" s="72">
+        <v>20</v>
+      </c>
+      <c r="F19" s="69"/>
+      <c r="G19" s="73"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s" s="76">
+        <v>9</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" t="s" s="77">
+        <v>12</v>
+      </c>
+      <c r="D20" s="75"/>
+      <c r="E20" t="s" s="78">
+        <v>21</v>
+      </c>
+      <c r="F20" s="75"/>
+      <c r="G20" s="79"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s" s="82">
+        <v>9</v>
+      </c>
+      <c r="B21" s="81"/>
+      <c r="C21" t="s" s="83">
+        <v>10</v>
+      </c>
+      <c r="D21" s="81"/>
+      <c r="E21" t="s" s="84">
+        <v>22</v>
+      </c>
+      <c r="F21" s="81"/>
+      <c r="G21" s="85"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="88">
+        <v>9</v>
+      </c>
+      <c r="B22" s="87"/>
+      <c r="C22" t="s" s="89">
+        <v>12</v>
+      </c>
+      <c r="D22" s="87"/>
+      <c r="E22" t="s" s="90">
+        <v>23</v>
+      </c>
+      <c r="F22" s="87"/>
+      <c r="G22" s="91"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s" s="94">
+        <v>9</v>
+      </c>
+      <c r="B23" s="93"/>
+      <c r="C23" t="s" s="95">
+        <v>10</v>
+      </c>
+      <c r="D23" s="93"/>
+      <c r="E23" t="s" s="96">
+        <v>24</v>
+      </c>
+      <c r="F23" s="93"/>
+      <c r="G23" s="97"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s" s="100">
+        <v>9</v>
+      </c>
+      <c r="B24" s="99"/>
+      <c r="C24" t="s" s="101">
+        <v>12</v>
+      </c>
+      <c r="D24" s="99"/>
+      <c r="E24" t="s" s="102">
+        <v>25</v>
+      </c>
+      <c r="F24" s="99"/>
+      <c r="G24" s="103"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s" s="106">
+        <v>9</v>
+      </c>
+      <c r="B25" s="105"/>
+      <c r="C25" t="s" s="107">
+        <v>10</v>
+      </c>
+      <c r="D25" s="105"/>
+      <c r="E25" t="s" s="108">
+        <v>26</v>
+      </c>
+      <c r="F25" s="105"/>
+      <c r="G25" s="109"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s" s="112">
+        <v>9</v>
+      </c>
+      <c r="B26" s="111"/>
+      <c r="C26" t="s" s="113">
+        <v>12</v>
+      </c>
+      <c r="D26" s="111"/>
+      <c r="E26" t="s" s="114">
+        <v>27</v>
+      </c>
+      <c r="F26" s="111"/>
+      <c r="G26" s="115"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="116"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>